<commit_message>
add freq pbmc/lymph plots
</commit_message>
<xml_diff>
--- a/explore/openCyto/compManual/match.xlsx
+++ b/explore/openCyto/compManual/match.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="4640" windowWidth="26860" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="820" yWindow="2340" windowWidth="26860" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="219">
   <si>
     <t>ABBREVIATION</t>
   </si>
@@ -476,9 +476,6 @@
     <t>MapManual</t>
   </si>
   <si>
-    <t>ParentMatch</t>
-  </si>
-  <si>
     <t>NaiveB</t>
   </si>
   <si>
@@ -546,13 +543,154 @@
   </si>
   <si>
     <t>Tcell</t>
+  </si>
+  <si>
+    <t>PBMCs (SSC-A v FSC-A) (FSC-A (FSC-A) v SSC-A (SSC-A))</t>
+  </si>
+  <si>
+    <t>Single Cells (FSC-H v FSC-W) (FSC-W (FSC-W) v FSC-H (FSC-H))</t>
+  </si>
+  <si>
+    <t>Live PBMCs (PE- CD45+) (Comp-PE-A (L/D) v Comp-APC-Cy7-A (CD45))</t>
+  </si>
+  <si>
+    <t>Live cells (PE-) (Comp-PE-A (L/D) v SSC-A (SSC-A))</t>
+  </si>
+  <si>
+    <t>naive helper Tcells (CD95-, CD28+) (Comp-BV 605-A (CD95) v Comp-BV 510-A (CD28))</t>
+  </si>
+  <si>
+    <t>naive cytotoxic Tcells (CD95- CD28+) (Comp-BV 605-A (CD95) v Comp-BV 510-A (CD28))</t>
+  </si>
+  <si>
+    <t>central memory helper Tcells (CD95+, CD28+) (Comp-BV 605-A (CD95) v Comp-BV 510-A (CD28))</t>
+  </si>
+  <si>
+    <t>effector memory helper Tcells (CD95+, CD28-) (Comp-BV 605-A (CD95) v Comp-BV 510-A (CD28))</t>
+  </si>
+  <si>
+    <t>naive cytotoxic Tcells (CCR7+ , CD45RA+) (Comp-BV 421-A (CCR7) v Comp-BV 711-A (CD45RA))</t>
+  </si>
+  <si>
+    <t>central memory cytotoxic Tcells (CD95+ CD28+) (Comp-BV 605-A (CD95) v Comp-BV 510-A (CD28))</t>
+  </si>
+  <si>
+    <t>effector memory cytotoxic Tcells (CD95+ CD28-) (Comp-BV 605-A (CD95) v Comp-BV 510-A (CD28))</t>
+  </si>
+  <si>
+    <t>cytotoxic Tcells CD27- , CD28+ (Comp-BB515-A (CD27) v Comp-BV 510-A (CD28))</t>
+  </si>
+  <si>
+    <t>JflowMatch</t>
+  </si>
+  <si>
+    <t>B cells (CD3MINUS CD19PLUS) (CompMINUSAPCMINUSA (CD3) v CompMINUSPEMINUSCy7MINUSA (CD19))</t>
+  </si>
+  <si>
+    <t>IgDPLUS memory Bcells (CD27PLUS) (CompMINUSBUV 737MINUSA (IgD) v CompMINUSBB515MINUSA (CD27))</t>
+  </si>
+  <si>
+    <t>IgDMINUS memory Bcells (CD27PLUS) (CompMINUSBUV 737MINUSA (IgD) v CompMINUSBB515MINUSA (CD27))</t>
+  </si>
+  <si>
+    <t>naive Bcells (CD27MINUS IgDPLUS) (CompMINUSBUV 737MINUSA (IgD) v CompMINUSBB515MINUSA (CD27))</t>
+  </si>
+  <si>
+    <t>Tcells (CD3PLUS CD19MINUS) (CompMINUSAPCMINUSA (CD3) v CompMINUSPEMINUSCy7MINUSA (CD19))</t>
+  </si>
+  <si>
+    <t>cytotoxic TcellsMINUSCD8PLUS (CompMINUSAPCMINUSCy7MINUSA (CD4) v CompMINUSBUV 395MINUSA (CD8))</t>
+  </si>
+  <si>
+    <t>activated cytotoxic Tcells (CD8PLUS HLAMINUSDRPLUS) (CompMINUSPEMINUSCF594MINUSA (HLAMINUSDR) v CompMINUSBUV 395MINUSA (CD8))</t>
+  </si>
+  <si>
+    <t>effector memory cytotoxic Tcells (CCR7MINUS , CD45RAMINUS) (CompMINUSBV 421MINUSA (CCR7) v CompMINUSBV 711MINUSA (CD45RA))</t>
+  </si>
+  <si>
+    <t>effector cytotoxic Tcells  (CCR7MINUS  CD45RAPLUS) (CompMINUSBV 421MINUSA (CCR7) v CompMINUSBV 711MINUSA (CD45RA))</t>
+  </si>
+  <si>
+    <t>pE cytotoxic Tcells (CD27MINUS  CD28MINUS) (CompMINUSBB515MINUSA (CD27) v CompMINUSBV 510MINUSA (CD28))</t>
+  </si>
+  <si>
+    <t>pE1 cytotoxic Tcells (CD27PLUS  CD28PLUS) (CompMINUSBB515MINUSA (CD27) v CompMINUSBV 510MINUSA (CD28))</t>
+  </si>
+  <si>
+    <t>pE2 cytotoxic Tcells (CD27PLUS , CD28MINUS) (CompMINUSBB515MINUSA (CD27) v CompMINUSBV 510MINUSA (CD28))</t>
+  </si>
+  <si>
+    <t>central memory cytotoxic Tcells (CCR7PLUS , CD45RAMINUS) (CompMINUSBV 421MINUSA (CCR7) v CompMINUSBV 711MINUSA (CD45RA))</t>
+  </si>
+  <si>
+    <t>EM1 cytotoxic Tcells (CD27PLUS  CD28PLUS) (CompMINUSBB515MINUSA (CD27) v CompMINUSBV 510MINUSA (CD28))</t>
+  </si>
+  <si>
+    <t>EM2 cytotoxic Tcells (CD27PLUS  CD28MINUS) (CompMINUSBB515MINUSA (CD27) v CompMINUSBV 510MINUSA (CD28))</t>
+  </si>
+  <si>
+    <t>EM3 cytotoxic Tcells (CD27MINUS  CD28MINUS) (CompMINUSBB515MINUSA (CD27) v CompMINUSBV 510MINUSA (CD28))</t>
+  </si>
+  <si>
+    <t>EM4 cytotoxic Tcells (CD27MINUS  CD28PLUS) (CompMINUSBB515MINUSA (CD27) v CompMINUSBV 510MINUSA (CD28))</t>
+  </si>
+  <si>
+    <t>naive helper Tcells (CCR7PLUS CD45RAPLUS) (CompMINUSBV 421MINUSA (CCR7) v CompMINUSBV 711MINUSA (CD45RA))</t>
+  </si>
+  <si>
+    <t>Helper TcellsMINUSCD4PLUS (CompMINUSAPCMINUSCy7MINUSA (CD4) v CompMINUSBUV 395MINUSA (CD8))</t>
+  </si>
+  <si>
+    <t>activated helper Tcells (CD4PLUS HLAMINUSDRPLUS) (CompMINUSPEMINUSCF594MINUSA (HLAMINUSDR) v CompMINUSAPCMINUSCy7MINUSA (CD4))</t>
+  </si>
+  <si>
+    <t>central memory helper Tcells (CCR7PLUS CD45RAMINUS) (CompMINUSBV 421MINUSA (CCR7) v CompMINUSBV 711MINUSA (CD45RA))</t>
+  </si>
+  <si>
+    <t>effector helper Tcells (CCR7MINUS CD45RAPLUS) (CompMINUSBV 421MINUSA (CCR7) v CompMINUSBV 711MINUSA (CD45RA))</t>
+  </si>
+  <si>
+    <t>effector memory helper Tcells (CCR7MINUS CD45RAMINUS) (CompMINUSBV 421MINUSA (CCR7) v CompMINUSBV 711MINUSA (CD45RA))</t>
+  </si>
+  <si>
+    <t>DC NK MONOCYTES (CD3MINUS CD19MINUS) (CompMINUSAPCMINUSA (CD3) v CompMINUSPEMINUSCy7MINUSA (CD19))</t>
+  </si>
+  <si>
+    <t>DC NK (CD20MINUS CD14MINUS) (CompMINUSBUV 395MINUSA (CD20) v CompMINUSBV 510MINUSA (CD14))</t>
+  </si>
+  <si>
+    <t>DC (HLAMINUSDRPLUS) (CompMINUSPEMINUSCF594MINUSA (HLAMINUSDR) v SSCMINUSA (SSCMINUSA))</t>
+  </si>
+  <si>
+    <t>Myeloid DC (CD11cPLUS CD123MINUS) (CompMINUSBB515MINUSA (CD11c) v CompMINUSBV 711MINUSA (CD123))</t>
+  </si>
+  <si>
+    <t>Plasmacytoid DC (CD11cMINUS CD123PLUS) (CompMINUSBB515MINUSA (CD11c) v CompMINUSBV 711MINUSA (CD123))</t>
+  </si>
+  <si>
+    <t>NK (CD16PLUS) (CompMINUSBUV 737MINUSA (CD16) v SSCMINUSA (SSCMINUSA))</t>
+  </si>
+  <si>
+    <t>NK CD56HI (CompMINUSBV 421MINUSA (CD56) v CompMINUSBUV 737MINUSA (CD16))</t>
+  </si>
+  <si>
+    <t>NK CD56LO (CompMINUSBV 421MINUSA (CD56) v CompMINUSBUV 737MINUSA (CD16))</t>
+  </si>
+  <si>
+    <t>MONOCYTES (CD20MINUS CD14PLUS) (CompMINUSBUV 395MINUSA (CD20) v CompMINUSBV 510MINUSA (CD14))</t>
+  </si>
+  <si>
+    <t>Classical monocytes (CD16MINUS CD14PLUS) (CompMINUSBUV 737MINUSA (CD16) v CompMINUSBV 510MINUSA (CD14))</t>
+  </si>
+  <si>
+    <t>Non classical monocytes (CD16PLUS CD14PLUS) (CompMINUSBUV 737MINUSA (CD16) v CompMINUSBV 510MINUSA (CD14))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -566,6 +704,29 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -585,10 +746,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -600,8 +769,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -877,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:Q72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -890,15 +1068,15 @@
     <col min="4" max="4" width="49.33203125" customWidth="1"/>
     <col min="5" max="5" width="28.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="42.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.83203125" customWidth="1"/>
+    <col min="8" max="13" width="29.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -916,10 +1094,13 @@
         <v>148</v>
       </c>
       <c r="H1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -941,17 +1122,19 @@
       <c r="G2" t="s">
         <v>115</v>
       </c>
-      <c r="H2" t="e">
-        <f>VLOOKUP(E2,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -968,17 +1151,19 @@
       <c r="G3" t="s">
         <v>135</v>
       </c>
-      <c r="H3" t="str">
-        <f>VLOOKUP(E3,A:A,1,FALSE)</f>
-        <v>Bcell</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
@@ -995,17 +1180,16 @@
       <c r="G4" t="s">
         <v>133</v>
       </c>
-      <c r="H4" t="str">
-        <f>VLOOKUP(E4,A:A,1,FALSE)</f>
-        <v>Bcell</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>16</v>
@@ -1022,17 +1206,16 @@
       <c r="G5" t="s">
         <v>134</v>
       </c>
-      <c r="H5" t="str">
-        <f>VLOOKUP(E5,A:A,1,FALSE)</f>
-        <v>Bcell</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
@@ -1049,12 +1232,11 @@
       <c r="G6" t="s">
         <v>136</v>
       </c>
-      <c r="H6" t="e">
-        <f>VLOOKUP(E6,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -1076,12 +1258,11 @@
       <c r="G7" t="s">
         <v>129</v>
       </c>
-      <c r="H7" t="e">
-        <f>VLOOKUP(E7,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1103,17 +1284,16 @@
       <c r="G8" t="s">
         <v>114</v>
       </c>
-      <c r="H8" t="e">
-        <f>VLOOKUP(E8,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>27</v>
@@ -1130,17 +1310,16 @@
       <c r="G9" t="s">
         <v>132</v>
       </c>
-      <c r="H9" t="e">
-        <f>VLOOKUP(E9,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>30</v>
@@ -1157,17 +1336,16 @@
       <c r="G10" t="s">
         <v>131</v>
       </c>
-      <c r="H10" t="e">
-        <f>VLOOKUP(E10,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>33</v>
@@ -1184,17 +1362,16 @@
       <c r="G11" t="s">
         <v>120</v>
       </c>
-      <c r="H11" t="e">
-        <f>VLOOKUP(E11,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>37</v>
@@ -1211,17 +1388,16 @@
       <c r="G12" t="s">
         <v>122</v>
       </c>
-      <c r="H12" t="e">
-        <f>VLOOKUP(E12,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>40</v>
@@ -1238,17 +1414,16 @@
       <c r="G13" t="s">
         <v>121</v>
       </c>
-      <c r="H13" t="e">
-        <f>VLOOKUP(E13,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>43</v>
@@ -1265,17 +1440,16 @@
       <c r="G14" t="s">
         <v>130</v>
       </c>
-      <c r="H14" t="e">
-        <f>VLOOKUP(E14,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>47</v>
@@ -1292,17 +1466,16 @@
       <c r="G15" t="s">
         <v>119</v>
       </c>
-      <c r="H15" t="e">
-        <f>VLOOKUP(E15,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>51</v>
@@ -1319,17 +1492,19 @@
       <c r="G16" t="s">
         <v>117</v>
       </c>
-      <c r="H16" t="e">
-        <f>VLOOKUP(E16,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>54</v>
@@ -1346,17 +1521,19 @@
       <c r="G17" t="s">
         <v>116</v>
       </c>
-      <c r="H17" t="e">
-        <f>VLOOKUP(E17,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>57</v>
@@ -1373,17 +1550,16 @@
       <c r="G18" t="s">
         <v>118</v>
       </c>
-      <c r="H18" t="e">
-        <f>VLOOKUP(E18,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>60</v>
@@ -1400,12 +1576,11 @@
       <c r="G19" t="s">
         <v>127</v>
       </c>
-      <c r="H19" t="e">
-        <f>VLOOKUP(E19,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -1427,17 +1602,16 @@
       <c r="G20" t="s">
         <v>123</v>
       </c>
-      <c r="H20" t="e">
-        <f>VLOOKUP(E20,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>66</v>
@@ -1454,17 +1628,16 @@
       <c r="G21" t="s">
         <v>113</v>
       </c>
-      <c r="H21" t="e">
-        <f>VLOOKUP(E21,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>69</v>
@@ -1481,17 +1654,16 @@
       <c r="G22" t="s">
         <v>126</v>
       </c>
-      <c r="H22" t="e">
-        <f>VLOOKUP(E22,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>72</v>
@@ -1508,17 +1680,16 @@
       <c r="G23" t="s">
         <v>125</v>
       </c>
-      <c r="H23" t="e">
-        <f>VLOOKUP(E23,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>75</v>
@@ -1535,17 +1706,16 @@
       <c r="G24" t="s">
         <v>124</v>
       </c>
-      <c r="H24" t="e">
-        <f>VLOOKUP(E24,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>78</v>
@@ -1562,17 +1732,19 @@
       <c r="G25" t="s">
         <v>128</v>
       </c>
-      <c r="H25" t="e">
-        <f>VLOOKUP(E25,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>80</v>
@@ -1589,17 +1761,21 @@
       <c r="G26" t="s">
         <v>144</v>
       </c>
-      <c r="H26" t="e">
-        <f>VLOOKUP(E26,A:A,1,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>84</v>
@@ -1616,12 +1792,14 @@
       <c r="G27" t="s">
         <v>140</v>
       </c>
-      <c r="H27" t="str">
-        <f>VLOOKUP(E27,A:A,1,FALSE)</f>
-        <v>DC NK MONO</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>86</v>
       </c>
@@ -1643,12 +1821,11 @@
       <c r="G28" t="s">
         <v>143</v>
       </c>
-      <c r="H28" t="str">
-        <f>VLOOKUP(E28,A:A,1,FALSE)</f>
-        <v>DC NK</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
@@ -1670,12 +1847,11 @@
       <c r="G29" t="s">
         <v>138</v>
       </c>
-      <c r="H29" t="str">
-        <f>VLOOKUP(E29,A:A,1,FALSE)</f>
-        <v>DC</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
@@ -1697,12 +1873,14 @@
       <c r="G30" t="s">
         <v>137</v>
       </c>
-      <c r="H30" t="str">
-        <f>VLOOKUP(E30,A:A,1,FALSE)</f>
-        <v>DC</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>95</v>
       </c>
@@ -1724,12 +1902,14 @@
       <c r="G31" t="s">
         <v>146</v>
       </c>
-      <c r="H31" t="str">
-        <f>VLOOKUP(E31,A:A,1,FALSE)</f>
-        <v>DC NK</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>98</v>
       </c>
@@ -1751,12 +1931,14 @@
       <c r="G32" t="s">
         <v>141</v>
       </c>
-      <c r="H32" t="str">
-        <f>VLOOKUP(E32,A:A,1,FALSE)</f>
-        <v>NK</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>101</v>
       </c>
@@ -1778,12 +1960,11 @@
       <c r="G33" t="s">
         <v>139</v>
       </c>
-      <c r="H33" t="str">
-        <f>VLOOKUP(E33,A:A,1,FALSE)</f>
-        <v>NK</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>104</v>
       </c>
@@ -1805,12 +1986,11 @@
       <c r="G34" t="s">
         <v>145</v>
       </c>
-      <c r="H34" t="str">
-        <f>VLOOKUP(E34,A:A,1,FALSE)</f>
-        <v>DC NK MONO</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>107</v>
       </c>
@@ -1832,12 +2012,11 @@
       <c r="G35" t="s">
         <v>142</v>
       </c>
-      <c r="H35" t="str">
-        <f>VLOOKUP(E35,A:A,1,FALSE)</f>
-        <v>MONO</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>110</v>
       </c>
@@ -1859,9 +2038,143 @@
       <c r="G36" t="s">
         <v>147</v>
       </c>
-      <c r="H36" t="str">
-        <f>VLOOKUP(E36,A:A,1,FALSE)</f>
-        <v>MONO</v>
+      <c r="H36" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q41" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q42" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q43" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q45" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q46" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q49" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="53" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q53" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="54" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q59" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="60" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q60" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="61" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q61" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q62" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q63" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q64" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q65" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q66" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="67" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q68" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q69" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q70" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q71" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="17:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q72" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>